<commit_message>
Added a state outline
</commit_message>
<xml_diff>
--- a/FinalProject2019WhatIfScoring.xlsx
+++ b/FinalProject2019WhatIfScoring.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\classes\442\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coryjohns/Desktop/School/CSCI/csci442_final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C08FD9B1-24E7-4142-885E-9B589609D1C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{51D3C948-87F6-4BF8-8A5F-5B2C7F5CBF6D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -111,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,21 +462,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65E7488-60DF-42E2-9692-8F7D83BD4181}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>18</v>
       </c>
@@ -485,7 +487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -500,7 +502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,25 +511,31 @@
       </c>
       <c r="D4">
         <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4">
         <f>IF(F4=1,D4,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="G5">
         <f t="shared" ref="G5:G18" si="1">IF(F5=1,D5,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -545,7 +553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -563,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -578,7 +586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -593,7 +601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -608,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -623,19 +631,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -653,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -668,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -677,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -692,19 +703,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
       <c r="G17">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -716,36 +730,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="D21">
         <v>10</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
       <c r="G21">
         <f t="shared" ref="G21" si="2">IF(F21=1,D21,0)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="D23">
         <v>-4</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
       <c r="G23">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+        <f>IF(F23=1,D23,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -755,10 +764,10 @@
       </c>
       <c r="G26">
         <f>SUM(G3:G24)</f>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>24</v>
       </c>

</xml_diff>